<commit_message>
Misc changes, progress in excel file
</commit_message>
<xml_diff>
--- a/List of Facts.xlsx
+++ b/List of Facts.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
@@ -239,7 +239,7 @@
     <t xml:space="preserve">St Basil’s Cathedral</t>
   </si>
   <si>
-    <t xml:space="preserve">Picture of python</t>
+    <t xml:space="preserve">Picture of Elephant</t>
   </si>
   <si>
     <t xml:space="preserve">Russia ethnic makeup bar chart</t>
@@ -251,7 +251,7 @@
     <t xml:space="preserve">coastal border bar chart – top 10 countries</t>
   </si>
   <si>
-    <t xml:space="preserve">Bar chart of coastal borders of north American countries</t>
+    <t xml:space="preserve">Bar chart of coastal borders of Asian countries</t>
   </si>
   <si>
     <t xml:space="preserve">Map of St. Petersburg</t>
@@ -269,19 +269,19 @@
     <t xml:space="preserve">Map of Northern and Southern Hemispheres w/ coastal borders highlighted</t>
   </si>
   <si>
-    <t xml:space="preserve">Swaziland only borders one country</t>
+    <t xml:space="preserve">Swaziland (Eswatini) only borders one country</t>
   </si>
   <si>
     <t xml:space="preserve">Picture of the king of swaziland</t>
   </si>
   <si>
-    <t xml:space="preserve">Picture of the Washington Monument</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bar Chart of exports of Swaziland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bar chart of exports of Canada</t>
+    <t xml:space="preserve">Picture of a hockey player</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bar chart of age of residents of Eswatini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bar chart of age of residents of Canada</t>
   </si>
   <si>
     <t xml:space="preserve">Bar chart of coastal and land borders of Swaziland</t>
@@ -311,7 +311,7 @@
     <t xml:space="preserve">Picture of the black sea coastline</t>
   </si>
   <si>
-    <t xml:space="preserve">Picture of the Mississippi river</t>
+    <t xml:space="preserve">Picture of the Nile river</t>
   </si>
   <si>
     <t xml:space="preserve">Salinity of bodies of water</t>
@@ -746,12 +746,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -777,24 +777,24 @@
   </sheetPr>
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="N11" activeCellId="0" sqref="N11"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="4" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="1" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="28.7551020408163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="1" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="28.3469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1127,7 +1127,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="44.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>61</v>
       </c>
@@ -1139,41 +1139,41 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="K9" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="L9" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="M9" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="N9" s="3" t="s">
+      <c r="N9" s="8" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="35.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>73</v>
       </c>
@@ -1185,41 +1185,41 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="K10" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="L10" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="M10" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="N10" s="3" t="s">
+      <c r="N10" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="35.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>85</v>
       </c>
@@ -1231,16 +1231,16 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="8" t="s">
         <v>89</v>
       </c>
       <c r="H11" s="3" t="s">
@@ -1249,7 +1249,7 @@
       <c r="I11" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="J11" s="12" t="s">
+      <c r="J11" s="11" t="s">
         <v>92</v>
       </c>
       <c r="K11" s="1" t="s">
@@ -1369,7 +1369,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="12" t="s">
         <v>122</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -1571,12 +1571,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="29.5612244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="12" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="12" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="12" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="11" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="11" width="29.1581632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="7" min="4" style="11" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="11" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="11" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1600,7 +1600,7 @@
       <c r="J1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="n">
+      <c r="A2" s="11" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1622,7 +1622,7 @@
       <c r="J2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="n">
+      <c r="A3" s="11" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1644,7 +1644,7 @@
       <c r="J3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="n">
+      <c r="A4" s="11" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1670,7 +1670,7 @@
       <c r="J4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="n">
+      <c r="A5" s="11" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1712,7 +1712,7 @@
       <c r="J6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="n">
+      <c r="A7" s="11" t="n">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1734,7 +1734,7 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="n">
+      <c r="A8" s="11" t="n">
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1756,7 +1756,7 @@
       <c r="J8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="n">
+      <c r="A9" s="11" t="n">
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">

</xml_diff>

<commit_message>
Belgium facts - incomplete
</commit_message>
<xml_diff>
--- a/List of Facts.xlsx
+++ b/List of Facts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -784,21 +784,21 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="4" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L12" activeCellId="0" sqref="L12"/>
+      <selection pane="bottomLeft" activeCell="P24" activeCellId="0" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="27.4030612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1499,7 +1499,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="46.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>157</v>
       </c>
@@ -1511,37 +1511,37 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="I17" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="J17" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="K17" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="L17" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="M17" s="1" t="s">
+      <c r="M17" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="N17" s="1" t="s">
+      <c r="N17" s="9" t="s">
         <v>168</v>
       </c>
     </row>
@@ -1575,12 +1575,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="14" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="14" width="27.9438775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="14" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="14" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="14" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="14" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="14" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="14" width="27.6734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="14" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="4" style="14" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="14" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="14" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Belgium fact... done with facts!!! yay!
</commit_message>
<xml_diff>
--- a/List of Facts.xlsx
+++ b/List of Facts.xlsx
@@ -416,10 +416,10 @@
     <t xml:space="preserve">Over 95% of Belgium’s population lives in Urban areas</t>
   </si>
   <si>
-    <t xml:space="preserve">Picture of Antwerp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Picture of pencil</t>
+    <t xml:space="preserve">Picture of Brussels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Picture of Coliseum</t>
   </si>
   <si>
     <t xml:space="preserve">Population distribution of Belgium</t>
@@ -701,7 +701,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -750,10 +750,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -782,9 +778,9 @@
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="4" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="P24" activeCellId="0" sqref="P24"/>
+      <selection pane="bottomLeft" activeCell="M14" activeCellId="0" sqref="L14:M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1361,7 +1357,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="35.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
         <v>121</v>
       </c>
@@ -1373,34 +1369,34 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="I14" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="J14" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="K14" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="L14" s="3" t="s">
+      <c r="L14" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="M14" s="3" t="s">
+      <c r="M14" s="8" t="s">
         <v>131</v>
       </c>
       <c r="N14" s="3" t="s">
@@ -1503,11 +1499,11 @@
       <c r="A17" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B17" s="13" t="n">
+      <c r="B17" s="12" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="C17" s="13" t="n">
+      <c r="C17" s="12" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1550,7 +1546,6 @@
     <hyperlink ref="D8" r:id="rId1" display="Picture of waterfall in paraguay"/>
     <hyperlink ref="D11" r:id="rId2" display="Picture of the black sea coastline"/>
     <hyperlink ref="J11" r:id="rId3" display="Ancient map of the Black Sea"/>
-    <hyperlink ref="D14" r:id="rId4" display="Picture of Antwerp"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -1570,17 +1565,17 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
+      <selection pane="topLeft" activeCell="I11" activeCellId="1" sqref="L14:M14 I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="14" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="14" width="27.6734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="14" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="14" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="14" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="14" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="27.6734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="4" style="13" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="13" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="13" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1604,7 +1599,7 @@
       <c r="J1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="n">
+      <c r="A2" s="13" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1626,7 +1621,7 @@
       <c r="J2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14" t="n">
+      <c r="A3" s="13" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1648,7 +1643,7 @@
       <c r="J3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="14" t="n">
+      <c r="A4" s="13" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1674,7 +1669,7 @@
       <c r="J4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14" t="n">
+      <c r="A5" s="13" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1716,7 +1711,7 @@
       <c r="J6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="n">
+      <c r="A7" s="13" t="n">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1738,7 +1733,7 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="n">
+      <c r="A8" s="13" t="n">
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1760,7 +1755,7 @@
       <c r="J8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="14" t="n">
+      <c r="A9" s="13" t="n">
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">

</xml_diff>